<commit_message>
Finished BOM file for M6-RF315.
</commit_message>
<xml_diff>
--- a/hardware/M6-RF315/M6-RF315_BOM.xlsx
+++ b/hardware/M6-RF315/M6-RF315_BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
   <si>
     <t>Item #</t>
   </si>
@@ -90,6 +90,9 @@
     <t>Total Cost</t>
   </si>
   <si>
+    <t>Murata</t>
+  </si>
+  <si>
     <t>TDK</t>
   </si>
   <si>
@@ -117,12 +120,30 @@
     <t>Rohm</t>
   </si>
   <si>
+    <t>MCR03EZPFX1003</t>
+  </si>
+  <si>
+    <t>RHM100KHCT-ND</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1/10W 1% 0603 SMD</t>
+  </si>
+  <si>
     <t>Keystone</t>
   </si>
   <si>
     <t>TESTPOINT-GREEN</t>
   </si>
   <si>
+    <t>5121K-ND</t>
+  </si>
+  <si>
+    <t>TEST POINT PC COMPACT T/H GREEN</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16.000 MHZ 8PF SMD</t>
+  </si>
+  <si>
     <t>Total</t>
   </si>
   <si>
@@ -159,9 +180,6 @@
     <t>33nH</t>
   </si>
   <si>
-    <t>L0603</t>
-  </si>
-  <si>
     <t>L3</t>
   </si>
   <si>
@@ -246,10 +264,148 @@
     <t>Antenna Factor</t>
   </si>
   <si>
-    <t>ANT-315-CW-RH</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>C1608C0G1H120J</t>
+  </si>
+  <si>
+    <t>445-1270-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 12PF 50V 5% NP0 0603</t>
+  </si>
+  <si>
+    <t>C1608C0G1H150J</t>
+  </si>
+  <si>
+    <t>445-1271-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 15PF 50V 5% NP0 0603</t>
+  </si>
+  <si>
+    <t>C1608C0G1H6R8C</t>
+  </si>
+  <si>
+    <t>445-5038-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 6.8PF 50V NP0 0603</t>
+  </si>
+  <si>
+    <t>C1608C0G1H221J</t>
+  </si>
+  <si>
+    <t>445-1285-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 220PF 50V 5% NP0 0603</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF5602V</t>
+  </si>
+  <si>
+    <t>P56.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>RES 56.0K OHM 1/10W 1% 0603 SMD</t>
+  </si>
+  <si>
+    <t>Panasonic-ECG</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ511</t>
+  </si>
+  <si>
+    <t>RES 510 OHM 1/5W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>RHM510DCT-ND</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ131</t>
+  </si>
+  <si>
+    <t>RHM130DCT-ND</t>
+  </si>
+  <si>
+    <t>RES 130 OHM 1/5W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>296-21981-1-ND</t>
+  </si>
+  <si>
+    <t>IC RF TXRX LP SUB-IGHZ 20-QFN</t>
+  </si>
+  <si>
+    <t>NX3225GA-16.000M-STD-CRG-1</t>
+  </si>
+  <si>
+    <t>644-1157-1-ND</t>
+  </si>
+  <si>
+    <t>LQG15HS33NJ02D</t>
+  </si>
+  <si>
+    <t>490-2629-1-ND</t>
+  </si>
+  <si>
+    <t>INDUCTOR 33NH 200MA 0402</t>
+  </si>
+  <si>
+    <t>L0402</t>
+  </si>
+  <si>
+    <t>LQG15HS18NJ02D</t>
+  </si>
+  <si>
+    <t>490-2626-1-ND</t>
+  </si>
+  <si>
+    <t>INDUCTOR 18NH 300MA 0402</t>
+  </si>
+  <si>
+    <t>ANT-315-CW-RH-SMA</t>
+  </si>
+  <si>
+    <t>ANT-315-CW-RH-SMA-ND</t>
+  </si>
+  <si>
+    <t>ANTENNA 315MHZ 1/4WAVE SMA</t>
+  </si>
+  <si>
+    <t>5008K-ND</t>
+  </si>
+  <si>
+    <t>TEST POINT PC COMPACT .063"D ORN</t>
+  </si>
+  <si>
+    <t>APT1608MGC</t>
+  </si>
+  <si>
+    <t>754-1118-1-ND</t>
+  </si>
+  <si>
+    <t>LED 1.6X0.8MM 570NM GRN CLR SMD</t>
+  </si>
+  <si>
+    <t>APT1608SECK</t>
+  </si>
+  <si>
+    <t>754-1120-1-ND</t>
+  </si>
+  <si>
+    <t>LED 1.6X0.8MM 601NM ORN CLR SMD</t>
+  </si>
+  <si>
+    <t>5-1814832-1</t>
+  </si>
+  <si>
+    <t>A97594-ND</t>
+  </si>
+  <si>
+    <t>CONN SOCKET SMA STR DIE CAST PCB</t>
   </si>
 </sst>
 </file>
@@ -709,7 +865,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,13 +927,13 @@
         <v>9</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>23</v>
@@ -788,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -797,19 +953,19 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J4" s="2">
         <v>6</v>
@@ -831,23 +987,34 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="G5" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" t="s">
+        <v>85</v>
       </c>
       <c r="J5" s="2">
         <v>2</v>
+      </c>
+      <c r="K5">
+        <v>0.1</v>
       </c>
       <c r="L5" s="2">
         <f>J5*$C$25</f>
@@ -855,7 +1022,7 @@
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -863,23 +1030,34 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="G6" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I6" t="s">
+        <v>88</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0.1</v>
       </c>
       <c r="L6" s="2">
         <f>J6*$C$25</f>
@@ -887,7 +1065,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -895,23 +1073,34 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
       </c>
       <c r="J7" s="2">
         <v>3</v>
+      </c>
+      <c r="K7">
+        <v>0.13</v>
       </c>
       <c r="L7" s="2">
         <f>J7*$C$25</f>
@@ -919,7 +1108,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -927,23 +1116,34 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>94</v>
       </c>
       <c r="J8" s="2">
         <v>2</v>
+      </c>
+      <c r="K8">
+        <v>0.18</v>
       </c>
       <c r="L8" s="2">
         <f>J8*$C$25</f>
@@ -951,7 +1151,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -959,23 +1159,34 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" t="s">
+        <v>111</v>
       </c>
       <c r="J9" s="2">
         <v>3</v>
+      </c>
+      <c r="K9">
+        <v>0.17599999999999999</v>
       </c>
       <c r="L9" s="2">
         <f>J9*$C$25</f>
@@ -983,7 +1194,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5839999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -991,23 +1202,34 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" t="s">
+        <v>115</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0.17599999999999999</v>
       </c>
       <c r="L10" s="2">
         <f>J10*$C$25</f>
@@ -1015,7 +1237,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.52800000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1023,23 +1245,34 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
       </c>
       <c r="J11" s="2">
         <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0.16</v>
       </c>
       <c r="L11" s="2">
         <f>J11*$C$25</f>
@@ -1047,7 +1280,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1055,23 +1288,34 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" t="s">
+        <v>123</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0.56000000000000005</v>
       </c>
       <c r="L12" s="2">
         <f>J12*$C$25</f>
@@ -1079,7 +1323,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6800000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1090,20 +1334,31 @@
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" t="s">
+        <v>41</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0.94</v>
       </c>
       <c r="L13" s="2">
         <f>J13*$C$25</f>
@@ -1111,7 +1366,7 @@
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.82</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1119,23 +1374,34 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5008</v>
+      </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" t="s">
+        <v>120</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0.36</v>
       </c>
       <c r="L14" s="2">
         <f>J14*$C$25</f>
@@ -1143,7 +1409,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1151,23 +1417,34 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5121</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15" t="s">
+        <v>40</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0.38</v>
       </c>
       <c r="L15" s="2">
         <f>J15*$C$25</f>
@@ -1175,7 +1452,7 @@
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.1400000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1183,23 +1460,34 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" t="s">
+        <v>97</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0.04</v>
       </c>
       <c r="L16" s="2">
         <f>J16*$C$25</f>
@@ -1207,7 +1495,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1224,14 +1512,25 @@
         <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>36</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
+      </c>
+      <c r="K17">
+        <v>2.3E-2</v>
       </c>
       <c r="L17" s="2">
         <f>J17*$C$25</f>
@@ -1239,7 +1538,7 @@
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1247,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2">
         <v>500</v>
@@ -1256,14 +1555,25 @@
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I18" t="s">
+        <v>100</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
+      </c>
+      <c r="K18">
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L18" s="2">
         <f>J18*$C$25</f>
@@ -1271,7 +1581,7 @@
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.249</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1279,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2">
         <v>130</v>
@@ -1288,14 +1598,25 @@
         <v>16</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" t="s">
+        <v>104</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
+      </c>
+      <c r="K19">
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="L19" s="2">
         <f>J19*$C$25</f>
@@ -1303,37 +1624,48 @@
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>17</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="2">
-        <v>1</v>
-      </c>
-      <c r="L20" s="2">
+      <c r="K20" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="L20" s="3">
         <f>J20*$C$25</f>
-        <v>3</v>
-      </c>
-      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="M20" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1346,39 +1678,39 @@
         <v>12</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J21" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" s="4">
         <v>5.74</v>
       </c>
       <c r="L21" s="3">
         <f>J21*$C$25</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M21" s="4">
         <f>L21*K21</f>
-        <v>17.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1389,20 +1721,31 @@
         <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I22" t="s">
+        <v>129</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
+      </c>
+      <c r="K22">
+        <v>2.85</v>
       </c>
       <c r="L22" s="2">
         <f>J22*$C$25</f>
@@ -1410,7 +1753,7 @@
       </c>
       <c r="M22">
         <f>L22*K22</f>
-        <v>0</v>
+        <v>8.5500000000000007</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1418,25 +1761,34 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I23" t="s">
+        <v>118</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
+      </c>
+      <c r="K23">
+        <v>6.52</v>
       </c>
       <c r="L23" s="2">
         <f>J23*$C$25</f>
@@ -1444,7 +1796,7 @@
       </c>
       <c r="M23">
         <f>L23*K23</f>
-        <v>0</v>
+        <v>19.559999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1457,21 +1809,25 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C25" s="7">
         <v>3</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="J25" s="2">
         <f>SUM(J4:J24)</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L25">
         <f>SUM(L4:L24)</f>
-        <v>93</v>
+        <v>87</v>
+      </c>
+      <c r="M25">
+        <f>SUM(M4:M23)</f>
+        <v>42.698999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor corrections to BOM file.
</commit_message>
<xml_diff>
--- a/hardware/M6-RF315/M6-RF315_BOM.xlsx
+++ b/hardware/M6-RF315/M6-RF315_BOM.xlsx
@@ -84,9 +84,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>Bill of Materials for 'Marote - Power Supply Board (Rev A)'</t>
-  </si>
-  <si>
     <t>Total Cost</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>CONN SOCKET SMA STR DIE CAST PCB</t>
+  </si>
+  <si>
+    <t>Bill of Materials for 'Marote - M6-RF315 (Rev A)'</t>
   </si>
 </sst>
 </file>
@@ -865,7 +865,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>22</v>
+        <v>129</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -927,16 +927,16 @@
         <v>9</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -953,19 +953,19 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" t="s">
         <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
       </c>
       <c r="J4" s="2">
         <v>6</v>
@@ -987,28 +987,28 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" t="s">
         <v>84</v>
-      </c>
-      <c r="I5" t="s">
-        <v>85</v>
       </c>
       <c r="J5" s="2">
         <v>2</v>
@@ -1030,28 +1030,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" t="s">
         <v>87</v>
-      </c>
-      <c r="I6" t="s">
-        <v>88</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
@@ -1073,28 +1073,28 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" t="s">
         <v>90</v>
-      </c>
-      <c r="I7" t="s">
-        <v>91</v>
       </c>
       <c r="J7" s="2">
         <v>3</v>
@@ -1116,28 +1116,28 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" t="s">
         <v>93</v>
-      </c>
-      <c r="I8" t="s">
-        <v>94</v>
       </c>
       <c r="J8" s="2">
         <v>2</v>
@@ -1159,28 +1159,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" t="s">
         <v>110</v>
-      </c>
-      <c r="I9" t="s">
-        <v>111</v>
       </c>
       <c r="J9" s="2">
         <v>3</v>
@@ -1202,28 +1202,28 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="D10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" t="s">
         <v>114</v>
-      </c>
-      <c r="I10" t="s">
-        <v>115</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
@@ -1245,28 +1245,28 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" t="s">
         <v>125</v>
-      </c>
-      <c r="I11" t="s">
-        <v>126</v>
       </c>
       <c r="J11" s="2">
         <v>1</v>
@@ -1288,28 +1288,28 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" t="s">
         <v>122</v>
-      </c>
-      <c r="I12" t="s">
-        <v>123</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -1334,25 +1334,25 @@
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="F13" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="I13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -1374,16 +1374,16 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="2">
         <v>5008</v>
@@ -1392,10 +1392,10 @@
         <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I14" t="s">
         <v>119</v>
-      </c>
-      <c r="I14" t="s">
-        <v>120</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1417,16 +1417,16 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="2">
         <v>5121</v>
@@ -1435,10 +1435,10 @@
         <v>13</v>
       </c>
       <c r="H15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" t="s">
         <v>39</v>
-      </c>
-      <c r="I15" t="s">
-        <v>40</v>
       </c>
       <c r="J15" s="2">
         <v>1</v>
@@ -1460,28 +1460,28 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" t="s">
         <v>96</v>
-      </c>
-      <c r="I16" t="s">
-        <v>97</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
@@ -1512,19 +1512,19 @@
         <v>16</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" t="s">
         <v>35</v>
-      </c>
-      <c r="I17" t="s">
-        <v>36</v>
       </c>
       <c r="J17" s="2">
         <v>1</v>
@@ -1546,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2">
         <v>500</v>
@@ -1555,19 +1555,19 @@
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I18" t="s">
         <v>99</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="I18" t="s">
-        <v>100</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -1589,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2">
         <v>130</v>
@@ -1598,19 +1598,19 @@
         <v>16</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" t="s">
         <v>103</v>
-      </c>
-      <c r="I19" t="s">
-        <v>104</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
@@ -1635,39 +1635,39 @@
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="J20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="4">
         <v>4.95</v>
       </c>
       <c r="L20" s="3">
         <f>J20*$C$25</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M20" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.850000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1678,39 +1678,39 @@
         <v>12</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="J21" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="4">
         <v>5.74</v>
       </c>
       <c r="L21" s="3">
         <f>J21*$C$25</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M21" s="4">
         <f>L21*K21</f>
-        <v>0</v>
+        <v>17.22</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1721,25 +1721,25 @@
         <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" t="s">
         <v>128</v>
-      </c>
-      <c r="I22" t="s">
-        <v>129</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
@@ -1761,28 +1761,28 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="F23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" t="s">
         <v>117</v>
-      </c>
-      <c r="I23" t="s">
-        <v>118</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
@@ -1809,25 +1809,25 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="7">
         <v>3</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J25" s="2">
         <f>SUM(J4:J24)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L25">
         <f>SUM(L4:L24)</f>
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="M25">
         <f>SUM(M4:M23)</f>
-        <v>42.698999999999998</v>
+        <v>74.769000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BOM and removed some DRC errors.
</commit_message>
<xml_diff>
--- a/hardware/M6-RF315/M6-RF315_BOM.xlsx
+++ b/hardware/M6-RF315/M6-RF315_BOM.xlsx
@@ -550,14 +550,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,20 +883,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -974,12 +974,12 @@
         <v>0.08</v>
       </c>
       <c r="L4" s="2">
-        <f>J4*$C$25</f>
-        <v>18</v>
+        <f t="shared" ref="L4:L23" si="0">J4*$C$25</f>
+        <v>12</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M20" si="0">L4*K4</f>
-        <v>1.44</v>
+        <f t="shared" ref="M4:M20" si="1">L4*K4</f>
+        <v>0.96</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1017,12 +1017,12 @@
         <v>0.1</v>
       </c>
       <c r="L5" s="2">
-        <f>J5*$C$25</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" si="1"/>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1060,12 +1060,12 @@
         <v>0.1</v>
       </c>
       <c r="L6" s="2">
-        <f>J6*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1103,12 +1103,12 @@
         <v>0.13</v>
       </c>
       <c r="L7" s="2">
-        <f>J7*$C$25</f>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
-        <v>1.17</v>
+        <f t="shared" si="1"/>
+        <v>0.78</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1146,12 +1146,12 @@
         <v>0.18</v>
       </c>
       <c r="L8" s="2">
-        <f>J8*$C$25</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
-        <v>1.08</v>
+        <f t="shared" si="1"/>
+        <v>0.72</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1189,12 +1189,12 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="L9" s="2">
-        <f>J9*$C$25</f>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
-        <v>1.5839999999999999</v>
+        <f t="shared" si="1"/>
+        <v>1.056</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1232,12 +1232,12 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="L10" s="2">
-        <f>J10*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M10">
-        <f t="shared" si="0"/>
-        <v>0.52800000000000002</v>
+        <f t="shared" si="1"/>
+        <v>0.35199999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1275,12 +1275,12 @@
         <v>0.16</v>
       </c>
       <c r="L11" s="2">
-        <f>J11*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M11">
-        <f t="shared" si="0"/>
-        <v>0.48</v>
+        <f t="shared" si="1"/>
+        <v>0.32</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1318,12 +1318,12 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="L12" s="2">
-        <f>J12*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
-        <v>1.6800000000000002</v>
+        <f t="shared" si="1"/>
+        <v>1.1200000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1361,12 +1361,12 @@
         <v>0.94</v>
       </c>
       <c r="L13" s="2">
-        <f>J13*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
-        <v>2.82</v>
+        <f t="shared" si="1"/>
+        <v>1.88</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1404,12 +1404,12 @@
         <v>0.36</v>
       </c>
       <c r="L14" s="2">
-        <f>J14*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
-        <v>1.08</v>
+        <f t="shared" si="1"/>
+        <v>0.72</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1447,12 +1447,12 @@
         <v>0.38</v>
       </c>
       <c r="L15" s="2">
-        <f>J15*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M15">
-        <f t="shared" si="0"/>
-        <v>1.1400000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.76</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1490,12 +1490,12 @@
         <v>0.04</v>
       </c>
       <c r="L16" s="2">
-        <f>J16*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M16">
-        <f t="shared" si="0"/>
-        <v>0.12</v>
+        <f t="shared" si="1"/>
+        <v>0.08</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1533,12 +1533,12 @@
         <v>2.3E-2</v>
       </c>
       <c r="L17" s="2">
-        <f>J17*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M17">
-        <f t="shared" si="0"/>
-        <v>6.9000000000000006E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1576,12 +1576,12 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L18" s="2">
-        <f>J18*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M18">
-        <f t="shared" si="0"/>
-        <v>0.249</v>
+        <f t="shared" si="1"/>
+        <v>0.16600000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1619,12 +1619,12 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="L19" s="2">
-        <f>J19*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M19">
-        <f t="shared" si="0"/>
-        <v>0.249</v>
+        <f t="shared" si="1"/>
+        <v>0.16600000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1662,12 +1662,12 @@
         <v>4.95</v>
       </c>
       <c r="L20" s="3">
-        <f>J20*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" si="0"/>
-        <v>14.850000000000001</v>
+        <f t="shared" si="1"/>
+        <v>9.9</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1677,19 +1677,19 @@
       <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="9" t="s">
         <v>13</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -1698,19 +1698,19 @@
       <c r="I21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="9">
         <v>1</v>
       </c>
       <c r="K21" s="4">
         <v>5.74</v>
       </c>
       <c r="L21" s="3">
-        <f>J21*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M21" s="4">
         <f>L21*K21</f>
-        <v>17.22</v>
+        <v>11.48</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1748,12 +1748,12 @@
         <v>2.85</v>
       </c>
       <c r="L22" s="2">
-        <f>J22*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M22">
         <f>L22*K22</f>
-        <v>8.5500000000000007</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1791,12 +1791,12 @@
         <v>6.52</v>
       </c>
       <c r="L23" s="2">
-        <f>J23*$C$25</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="M23">
         <f>L23*K23</f>
-        <v>19.559999999999999</v>
+        <v>13.04</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1812,7 +1812,7 @@
         <v>77</v>
       </c>
       <c r="C25" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>41</v>
@@ -1823,11 +1823,11 @@
       </c>
       <c r="L25">
         <f>SUM(L4:L24)</f>
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="M25">
         <f>SUM(M4:M23)</f>
-        <v>74.769000000000005</v>
+        <v>49.846000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected the crystal part number in BOM from 16 MHz to 26 MHz.
</commit_message>
<xml_diff>
--- a/hardware/M6-RF315/M6-RF315_BOM.xlsx
+++ b/hardware/M6-RF315/M6-RF315_BOM.xlsx
@@ -138,9 +138,6 @@
     <t>TEST POINT PC COMPACT T/H GREEN</t>
   </si>
   <si>
-    <t>CRYSTAL 16.000 MHZ 8PF SMD</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -336,12 +333,6 @@
     <t>IC RF TXRX LP SUB-IGHZ 20-QFN</t>
   </si>
   <si>
-    <t>NX3225GA-16.000M-STD-CRG-1</t>
-  </si>
-  <si>
-    <t>644-1157-1-ND</t>
-  </si>
-  <si>
     <t>LQG15HS33NJ02D</t>
   </si>
   <si>
@@ -406,6 +397,15 @@
   </si>
   <si>
     <t>Bill of Materials for 'Marote - M6-RF315 (Rev A)'</t>
+  </si>
+  <si>
+    <t>CRYSTAL 26.000 MHZ 10PF SMD</t>
+  </si>
+  <si>
+    <t>NX3225GA-26MHZ-TI</t>
+  </si>
+  <si>
+    <t>644-1160-1-ND</t>
   </si>
 </sst>
 </file>
@@ -865,7 +865,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
@@ -927,13 +927,13 @@
         <v>9</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M3" s="5" t="s">
         <v>22</v>
@@ -944,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -987,10 +987,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -999,16 +999,16 @@
         <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" t="s">
         <v>83</v>
-      </c>
-      <c r="I5" t="s">
-        <v>84</v>
       </c>
       <c r="J5" s="2">
         <v>2</v>
@@ -1030,10 +1030,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -1042,16 +1042,16 @@
         <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" t="s">
         <v>86</v>
-      </c>
-      <c r="I6" t="s">
-        <v>87</v>
       </c>
       <c r="J6" s="2">
         <v>1</v>
@@ -1073,10 +1073,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -1085,16 +1085,16 @@
         <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" t="s">
         <v>89</v>
-      </c>
-      <c r="I7" t="s">
-        <v>90</v>
       </c>
       <c r="J7" s="2">
         <v>3</v>
@@ -1116,10 +1116,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1128,16 +1128,16 @@
         <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" t="s">
         <v>92</v>
-      </c>
-      <c r="I8" t="s">
-        <v>93</v>
       </c>
       <c r="J8" s="2">
         <v>2</v>
@@ -1159,28 +1159,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J9" s="2">
         <v>3</v>
@@ -1202,28 +1202,28 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J10" s="2">
         <v>1</v>
@@ -1251,22 +1251,22 @@
         <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J11" s="2">
         <v>1</v>
@@ -1288,28 +1288,28 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
@@ -1334,25 +1334,25 @@
         <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="F13" s="2" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="J13" s="2">
         <v>1</v>
@@ -1374,13 +1374,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>36</v>
@@ -1392,10 +1392,10 @@
         <v>13</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J14" s="2">
         <v>1</v>
@@ -1417,7 +1417,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
@@ -1460,28 +1460,28 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" t="s">
         <v>95</v>
-      </c>
-      <c r="I16" t="s">
-        <v>96</v>
       </c>
       <c r="J16" s="2">
         <v>1</v>
@@ -1546,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2">
         <v>500</v>
@@ -1558,16 +1558,16 @@
         <v>32</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" t="s">
         <v>98</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" t="s">
-        <v>99</v>
       </c>
       <c r="J18" s="2">
         <v>1</v>
@@ -1589,7 +1589,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2">
         <v>130</v>
@@ -1601,16 +1601,16 @@
         <v>32</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" t="s">
         <v>102</v>
-      </c>
-      <c r="I19" t="s">
-        <v>103</v>
       </c>
       <c r="J19" s="2">
         <v>1</v>
@@ -1635,25 +1635,25 @@
         <v>20</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>13</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>105</v>
       </c>
       <c r="J20" s="3">
         <v>1</v>
@@ -1678,25 +1678,25 @@
         <v>12</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="F21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="J21" s="9">
         <v>1</v>
@@ -1721,25 +1721,25 @@
         <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J22" s="2">
         <v>1</v>
@@ -1761,28 +1761,28 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J23" s="2">
         <v>1</v>
@@ -1809,13 +1809,13 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="7">
         <v>2</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J25" s="2">
         <f>SUM(J4:J24)</f>

</xml_diff>